<commit_message>
Imrpove documentation and another example
</commit_message>
<xml_diff>
--- a/examples/checking_selection/Results.xlsx
+++ b/examples/checking_selection/Results.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Fixed selection" sheetId="1" r:id="rId1"/>
+    <sheet name="Random selection" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Fixed selection'!$A$1:$F$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Population size</t>
   </si>
@@ -41,10 +42,22 @@
     <t>Dominance</t>
   </si>
   <si>
-    <t>Mean</t>
+    <t>Error</t>
   </si>
   <si>
-    <t>Error</t>
+    <t>Beta (dominance)</t>
+  </si>
+  <si>
+    <t>Mean heterozygosity</t>
+  </si>
+  <si>
+    <t>Location (mu)</t>
+  </si>
+  <si>
+    <t>scale (sigma)</t>
+  </si>
+  <si>
+    <t>shape (alpha)</t>
   </si>
 </sst>
 </file>
@@ -363,18 +376,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="24.08984375" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,13 +401,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -414,7 +427,7 @@
         <v>3.0880666786581098E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5000</v>
       </c>
@@ -434,7 +447,7 @@
         <v>3.08479280646132E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5000</v>
       </c>
@@ -454,7 +467,7 @@
         <v>6.9200698495276001E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5000</v>
       </c>
@@ -474,7 +487,7 @@
         <v>9.9799216863907194E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -495,7 +508,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5000</v>
       </c>
@@ -515,7 +528,7 @@
         <v>7.2661123937364199E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5000</v>
       </c>
@@ -535,7 +548,7 @@
         <v>7.7273373845205108E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5000</v>
       </c>
@@ -555,7 +568,7 @@
         <v>7.5273781025252601E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5000</v>
       </c>
@@ -575,7 +588,7 @@
         <v>7.5639170624286596E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5000</v>
       </c>
@@ -595,7 +608,7 @@
         <v>7.4190247175480204E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5000</v>
       </c>
@@ -615,7 +628,7 @@
         <v>7.4181704220865804E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5000</v>
       </c>
@@ -635,7 +648,7 @@
         <v>7.0501149497166902E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5000</v>
       </c>
@@ -655,7 +668,7 @@
         <v>7.0359105045374702E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5000</v>
       </c>
@@ -675,7 +688,7 @@
         <v>2.9969232390839898E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5000</v>
       </c>
@@ -693,6 +706,306 @@
       </c>
       <c r="F16">
         <v>3.1537204970038599E-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>500</v>
+      </c>
+      <c r="B17">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>-0.1</v>
+      </c>
+      <c r="E17">
+        <v>4.7901366428221699E-4</v>
+      </c>
+      <c r="F17">
+        <v>7.9186040568574796E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>500</v>
+      </c>
+      <c r="B18">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18">
+        <v>-0.01</v>
+      </c>
+      <c r="E18">
+        <v>4.7743277693964997E-3</v>
+      </c>
+      <c r="F18">
+        <v>8.44314691772678E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>500</v>
+      </c>
+      <c r="B19">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <v>-1E-3</v>
+      </c>
+      <c r="E19">
+        <v>2.12613662702145E-2</v>
+      </c>
+      <c r="F19">
+        <v>8.7667273444200402E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>500</v>
+      </c>
+      <c r="B20">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>-1E-4</v>
+      </c>
+      <c r="E20">
+        <v>2.2882082366146E-2</v>
+      </c>
+      <c r="F20">
+        <v>8.9165024385333297E-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>500</v>
+      </c>
+      <c r="B21">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>-1.0000000000000001E-5</v>
+      </c>
+      <c r="E21">
+        <v>2.29012355490157E-2</v>
+      </c>
+      <c r="F21">
+        <v>9.3507932697891695E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>500</v>
+      </c>
+      <c r="B22">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>-9.9999999999999995E-7</v>
+      </c>
+      <c r="E22">
+        <v>2.2899377791179201E-2</v>
+      </c>
+      <c r="F22">
+        <v>9.1334964005533897E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>500</v>
+      </c>
+      <c r="B23">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>-9.9999999999999995E-8</v>
+      </c>
+      <c r="E23">
+        <v>2.2900045874578299E-2</v>
+      </c>
+      <c r="F23">
+        <v>9.2165912759854796E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>500</v>
+      </c>
+      <c r="B24">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>2.2901275689195699E-2</v>
+      </c>
+      <c r="F24">
+        <v>9.70224683104708E-7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>500</v>
+      </c>
+      <c r="B25">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E25">
+        <v>2.2900351267073099E-2</v>
+      </c>
+      <c r="F25">
+        <v>9.2630906047031395E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>500</v>
+      </c>
+      <c r="B26">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E26">
+        <v>2.28993539802568E-2</v>
+      </c>
+      <c r="F26">
+        <v>9.5220398845031705E-7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>500</v>
+      </c>
+      <c r="B27">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E27">
+        <v>2.28987225237577E-2</v>
+      </c>
+      <c r="F27">
+        <v>9.2537308442433804E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>500</v>
+      </c>
+      <c r="B28">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>1E-4</v>
+      </c>
+      <c r="E28">
+        <v>2.28837442065658E-2</v>
+      </c>
+      <c r="F28">
+        <v>9.4431935442857899E-7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>500</v>
+      </c>
+      <c r="B29">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>1E-3</v>
+      </c>
+      <c r="E29">
+        <v>2.1262333934199799E-2</v>
+      </c>
+      <c r="F29">
+        <v>8.4254369700848895E-7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>500</v>
+      </c>
+      <c r="B30">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30">
+        <v>0.01</v>
+      </c>
+      <c r="E30">
+        <v>4.7725916614814699E-3</v>
+      </c>
+      <c r="F30">
+        <v>8.76539502409995E-7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>500</v>
+      </c>
+      <c r="B31">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31">
+        <v>0.1</v>
+      </c>
+      <c r="E31">
+        <v>4.78909931345358E-4</v>
+      </c>
+      <c r="F31">
+        <v>7.9103076519571197E-7</v>
       </c>
     </row>
   </sheetData>
@@ -703,4 +1016,71 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>500</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-7.7446099999999997E-5</v>
+      </c>
+      <c r="E2">
+        <v>1.2641400000000001E-5</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>2.28887227654875E-2</v>
+      </c>
+      <c r="H2">
+        <v>9.2671024847324002E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Another round of computation
</commit_message>
<xml_diff>
--- a/examples/checking_selection/Results.xlsx
+++ b/examples/checking_selection/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Fixed selection" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Population size</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Selection</t>
-  </si>
-  <si>
-    <t>Dominance</t>
   </si>
   <si>
     <t>Error</t>
@@ -376,18 +373,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -395,19 +392,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -415,7 +412,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>-0.1</v>
@@ -427,7 +424,7 @@
         <v>3.0880666786581098E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5000</v>
       </c>
@@ -435,7 +432,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>-0.01</v>
@@ -447,7 +444,7 @@
         <v>3.08479280646132E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5000</v>
       </c>
@@ -455,7 +452,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>-1E-3</v>
@@ -467,7 +464,7 @@
         <v>6.9200698495276001E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5000</v>
       </c>
@@ -475,7 +472,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>-1E-4</v>
@@ -487,7 +484,7 @@
         <v>9.9799216863907194E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -495,7 +492,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>-1.0000000000000001E-5</v>
@@ -508,7 +505,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5000</v>
       </c>
@@ -516,7 +513,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>-9.9999999999999995E-7</v>
@@ -528,7 +525,7 @@
         <v>7.2661123937364199E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5000</v>
       </c>
@@ -536,7 +533,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>-9.9999999999999995E-8</v>
@@ -548,7 +545,7 @@
         <v>7.7273373845205108E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5000</v>
       </c>
@@ -556,7 +553,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -568,7 +565,7 @@
         <v>7.5273781025252601E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5000</v>
       </c>
@@ -576,7 +573,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
         <v>9.9999999999999995E-8</v>
@@ -588,7 +585,7 @@
         <v>7.5639170624286596E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5000</v>
       </c>
@@ -596,7 +593,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D11" s="1">
         <v>9.9999999999999995E-7</v>
@@ -608,7 +605,7 @@
         <v>7.4190247175480204E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5000</v>
       </c>
@@ -616,7 +613,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <v>1.0000000000000001E-5</v>
@@ -628,7 +625,7 @@
         <v>7.4181704220865804E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>5000</v>
       </c>
@@ -636,7 +633,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>1E-4</v>
@@ -648,7 +645,7 @@
         <v>7.0501149497166902E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5000</v>
       </c>
@@ -656,7 +653,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>1E-3</v>
@@ -668,7 +665,7 @@
         <v>7.0359105045374702E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5000</v>
       </c>
@@ -676,7 +673,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D15" s="1">
         <v>0.01</v>
@@ -688,7 +685,7 @@
         <v>2.9969232390839898E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5000</v>
       </c>
@@ -696,7 +693,7 @@
         <v>1.1999999999999999E-6</v>
       </c>
       <c r="C16">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0.1</v>
@@ -708,7 +705,7 @@
         <v>3.1537204970038599E-7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>500</v>
       </c>
@@ -716,7 +713,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C17">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D17">
         <v>-0.1</v>
@@ -728,7 +725,7 @@
         <v>7.9186040568574796E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>500</v>
       </c>
@@ -736,7 +733,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>-0.01</v>
@@ -748,7 +745,7 @@
         <v>8.44314691772678E-7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>500</v>
       </c>
@@ -756,7 +753,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C19">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>-1E-3</v>
@@ -768,7 +765,7 @@
         <v>8.7667273444200402E-7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>500</v>
       </c>
@@ -776,7 +773,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>-1E-4</v>
@@ -788,7 +785,7 @@
         <v>8.9165024385333297E-7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>500</v>
       </c>
@@ -796,7 +793,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>-1.0000000000000001E-5</v>
@@ -808,7 +805,7 @@
         <v>9.3507932697891695E-7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>500</v>
       </c>
@@ -816,7 +813,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>-9.9999999999999995E-7</v>
@@ -828,7 +825,7 @@
         <v>9.1334964005533897E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>500</v>
       </c>
@@ -836,7 +833,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>-9.9999999999999995E-8</v>
@@ -848,7 +845,7 @@
         <v>9.2165912759854796E-7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>500</v>
       </c>
@@ -856,7 +853,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -868,7 +865,7 @@
         <v>9.70224683104708E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>500</v>
       </c>
@@ -876,7 +873,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>9.9999999999999995E-8</v>
@@ -888,7 +885,7 @@
         <v>9.2630906047031395E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>500</v>
       </c>
@@ -896,7 +893,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C26">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>9.9999999999999995E-7</v>
@@ -908,7 +905,7 @@
         <v>9.5220398845031705E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>500</v>
       </c>
@@ -916,7 +913,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C27">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <v>1.0000000000000001E-5</v>
@@ -928,7 +925,7 @@
         <v>9.2537308442433804E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>500</v>
       </c>
@@ -936,7 +933,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>1E-4</v>
@@ -948,7 +945,7 @@
         <v>9.4431935442857899E-7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>500</v>
       </c>
@@ -956,7 +953,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C29">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <v>1E-3</v>
@@ -968,7 +965,7 @@
         <v>8.4254369700848895E-7</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>500</v>
       </c>
@@ -976,7 +973,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C30">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>0.01</v>
@@ -988,7 +985,7 @@
         <v>8.76539502409995E-7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>500</v>
       </c>
@@ -996,7 +993,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="C31">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>0.1</v>
@@ -1006,6 +1003,306 @@
       </c>
       <c r="F31">
         <v>7.9103076519571197E-7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>500</v>
+      </c>
+      <c r="B32">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C32">
+        <v>3000</v>
+      </c>
+      <c r="D32">
+        <v>-0.1</v>
+      </c>
+      <c r="E32">
+        <v>4.1691982971239798E-3</v>
+      </c>
+      <c r="F32">
+        <v>9.2538903659896802E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>500</v>
+      </c>
+      <c r="B33">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C33">
+        <v>3000</v>
+      </c>
+      <c r="D33">
+        <v>-0.01</v>
+      </c>
+      <c r="E33">
+        <v>1.3055406069463101E-2</v>
+      </c>
+      <c r="F33">
+        <v>8.9620328805088196E-7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>500</v>
+      </c>
+      <c r="B34">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C34">
+        <v>3000</v>
+      </c>
+      <c r="D34">
+        <v>-1E-3</v>
+      </c>
+      <c r="E34">
+        <v>2.4496717223803598E-2</v>
+      </c>
+      <c r="F34">
+        <v>6.9501315400634595E-7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>500</v>
+      </c>
+      <c r="B35">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C35">
+        <v>3000</v>
+      </c>
+      <c r="D35">
+        <v>-1E-4</v>
+      </c>
+      <c r="E35">
+        <v>2.2934695456312101E-2</v>
+      </c>
+      <c r="F35">
+        <v>9.3995320417264996E-7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>500</v>
+      </c>
+      <c r="B36">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C36">
+        <v>3000</v>
+      </c>
+      <c r="D36">
+        <v>-1.0000000000000001E-5</v>
+      </c>
+      <c r="E36">
+        <v>2.2900342122981299E-2</v>
+      </c>
+      <c r="F36">
+        <v>8.89545545034269E-7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>500</v>
+      </c>
+      <c r="B37">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C37">
+        <v>3000</v>
+      </c>
+      <c r="D37">
+        <v>-9.9999999999999995E-7</v>
+      </c>
+      <c r="E37">
+        <v>2.2901792906144299E-2</v>
+      </c>
+      <c r="F37">
+        <v>9.0278389306826395E-7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>500</v>
+      </c>
+      <c r="B38">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C38">
+        <v>3000</v>
+      </c>
+      <c r="D38">
+        <v>-9.9999999999999995E-8</v>
+      </c>
+      <c r="E38">
+        <v>2.2900512274048299E-2</v>
+      </c>
+      <c r="F38">
+        <v>9.3071125576467297E-7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>500</v>
+      </c>
+      <c r="B39">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C39">
+        <v>3000</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>2.2901832709934799E-2</v>
+      </c>
+      <c r="F39">
+        <v>9.2693919052056203E-7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>500</v>
+      </c>
+      <c r="B40">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C40">
+        <v>3000</v>
+      </c>
+      <c r="D40">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="E40">
+        <v>2.2901341615610998E-2</v>
+      </c>
+      <c r="F40">
+        <v>9.3281368142378505E-7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>500</v>
+      </c>
+      <c r="B41">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C41">
+        <v>3000</v>
+      </c>
+      <c r="D41">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E41">
+        <v>2.2901628608370299E-2</v>
+      </c>
+      <c r="F41">
+        <v>9.3442116978865398E-7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>500</v>
+      </c>
+      <c r="B42">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C42">
+        <v>3000</v>
+      </c>
+      <c r="D42">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E42">
+        <v>2.29016409241166E-2</v>
+      </c>
+      <c r="F42">
+        <v>9.1087943935906605E-7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>500</v>
+      </c>
+      <c r="B43">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C43">
+        <v>3000</v>
+      </c>
+      <c r="D43">
+        <v>1E-4</v>
+      </c>
+      <c r="E43">
+        <v>2.2936721753343801E-2</v>
+      </c>
+      <c r="F43">
+        <v>9.4399012051949995E-7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>500</v>
+      </c>
+      <c r="B44">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C44">
+        <v>3000</v>
+      </c>
+      <c r="D44">
+        <v>1E-3</v>
+      </c>
+      <c r="E44">
+        <v>2.4495615406008101E-2</v>
+      </c>
+      <c r="F44">
+        <v>9.851769899301891E-7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>500</v>
+      </c>
+      <c r="B45">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C45">
+        <v>3000</v>
+      </c>
+      <c r="D45">
+        <v>0.01</v>
+      </c>
+      <c r="E45">
+        <v>1.3055848961001201E-2</v>
+      </c>
+      <c r="F45">
+        <v>8.9189702648256801E-7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>500</v>
+      </c>
+      <c r="B46">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C46">
+        <v>3000</v>
+      </c>
+      <c r="D46">
+        <v>0.1</v>
+      </c>
+      <c r="E46">
+        <v>4.1676133960321998E-3</v>
+      </c>
+      <c r="F46">
+        <v>9.0139796902327403E-7</v>
       </c>
     </row>
   </sheetData>
@@ -1020,15 +1317,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1036,25 +1337,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="H1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>500</v>
       </c>
@@ -1079,6 +1380,139 @@
       <c r="H2">
         <v>9.2671024847324002E-7</v>
       </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.2E-4</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>-7.7446099999999997E-5</v>
+      </c>
+      <c r="E3">
+        <v>1.2641400000000001E-5</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.162115210682967</v>
+      </c>
+      <c r="H3">
+        <v>9.5653370309104295E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>-7.7446099999999997E-5</v>
+      </c>
+      <c r="E4">
+        <v>1.2641400000000001E-5</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.41373653143983002</v>
+      </c>
+      <c r="H4">
+        <v>7.1585868134876596E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>-7.7446099999999997E-5</v>
+      </c>
+      <c r="E5">
+        <v>1.2641400000000001E-5</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2.2858246949783102E-2</v>
+      </c>
+      <c r="H5">
+        <v>9.2750913740357299E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.2E-5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-7.7446099999999997E-5</v>
+      </c>
+      <c r="E6">
+        <v>1.2641400000000001E-5</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.157511223990111</v>
+      </c>
+      <c r="H6">
+        <v>9.7069259292406307E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+      <c r="C7">
+        <v>3000</v>
+      </c>
+      <c r="D7">
+        <v>-0.13458587999999999</v>
+      </c>
+      <c r="E7">
+        <v>3.77358E-2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1.1842054593121901E-3</v>
+      </c>
+      <c r="H7">
+        <v>7.7324484217565303E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>